<commit_message>
mise à jour Gantt
</commit_message>
<xml_diff>
--- a/planning/gantt.xlsx
+++ b/planning/gantt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lesage Thibaut\Desktop\2324_INFOB318_Silver.Simon1\planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{371CA1B6-FD2D-4D97-9D69-B29B2E68DC71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D596E38A-662F-4919-83BF-D3F0CF0C6061}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
   <si>
     <t>…</t>
   </si>
@@ -77,6 +77,9 @@
   </si>
   <si>
     <t xml:space="preserve">Conception </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1ère Application To-Do List </t>
   </si>
 </sst>
 </file>
@@ -888,7 +891,7 @@
   <dimension ref="B2:AH46"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -978,7 +981,7 @@
       </c>
       <c r="I7" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J7" s="5">
         <f t="shared" si="0"/>
@@ -1218,7 +1221,7 @@
       </c>
       <c r="C9" s="22">
         <f>SUM(C10:C46)</f>
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="D9" s="26">
         <f>SUM(D10:D46)</f>
@@ -1242,7 +1245,7 @@
       </c>
       <c r="I9" s="26">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J9" s="26">
         <f t="shared" si="12"/>
@@ -1391,7 +1394,7 @@
       </c>
       <c r="C11" s="25">
         <f t="shared" ref="C11:C46" si="14">SUM(D11:AH11)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D11" s="17">
         <v>1</v>
@@ -1402,7 +1405,9 @@
       <c r="H11" s="12">
         <v>1</v>
       </c>
-      <c r="I11" s="12"/>
+      <c r="I11" s="12">
+        <v>1</v>
+      </c>
       <c r="J11" s="12"/>
       <c r="K11" s="12"/>
       <c r="L11" s="12"/>
@@ -1479,7 +1484,7 @@
       </c>
       <c r="C13" s="25">
         <f t="shared" si="14"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D13" s="17"/>
       <c r="E13" s="12">
@@ -1490,7 +1495,9 @@
       </c>
       <c r="G13" s="12"/>
       <c r="H13" s="12"/>
-      <c r="I13" s="12"/>
+      <c r="I13" s="12">
+        <v>2</v>
+      </c>
       <c r="J13" s="12"/>
       <c r="K13" s="12"/>
       <c r="L13" s="12"/>
@@ -1604,17 +1611,21 @@
       <c r="AH15" s="13"/>
     </row>
     <row r="16" spans="2:34" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="7"/>
+      <c r="B16" s="7" t="s">
+        <v>19</v>
+      </c>
       <c r="C16" s="25">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D16" s="17"/>
       <c r="E16" s="12"/>
       <c r="F16" s="12"/>
       <c r="G16" s="12"/>
       <c r="H16" s="12"/>
-      <c r="I16" s="12"/>
+      <c r="I16" s="12">
+        <v>2</v>
+      </c>
       <c r="J16" s="12"/>
       <c r="K16" s="12"/>
       <c r="L16" s="12"/>

</xml_diff>